<commit_message>
Group work - diary partial
</commit_message>
<xml_diff>
--- a/docs/Group Work Diary.xlsx
+++ b/docs/Group Work Diary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuzon\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Inventory-Managment-System\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C3F1A0-7246-4EEB-B0A4-79BC9172638C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA054F3A-44C0-4BC5-B666-EEDF581B7A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Group Diary" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>ItSE Group Work Diary Form</t>
   </si>
@@ -78,13 +78,121 @@
   </si>
   <si>
     <t>c3035956@student.shu.ac.uk</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Task Id</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Predecessor Task</t>
+  </si>
+  <si>
+    <t>Planned Start Date</t>
+  </si>
+  <si>
+    <t>Planned End Date</t>
+  </si>
+  <si>
+    <t>Actual Sart Date</t>
+  </si>
+  <si>
+    <t>Actual End Date</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Planning</t>
+  </si>
+  <si>
+    <t>Pln1</t>
+  </si>
+  <si>
+    <t>define scope</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Pln2</t>
+  </si>
+  <si>
+    <t>Use Case</t>
+  </si>
+  <si>
+    <t>Pln3</t>
+  </si>
+  <si>
+    <t>Pln4</t>
+  </si>
+  <si>
+    <t>ERD</t>
+  </si>
+  <si>
+    <t>WireFrames</t>
+  </si>
+  <si>
+    <t>Pln5</t>
+  </si>
+  <si>
+    <t>User Storeis + Acceptance Test</t>
+  </si>
+  <si>
+    <t>Define Scope</t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>Imp1</t>
+  </si>
+  <si>
+    <t>Imp2</t>
+  </si>
+  <si>
+    <t>Imp3</t>
+  </si>
+  <si>
+    <t>Imp4</t>
+  </si>
+  <si>
+    <t>Imp5</t>
+  </si>
+  <si>
+    <t>Imp6</t>
+  </si>
+  <si>
+    <t>Construct Database</t>
+  </si>
+  <si>
+    <t>Planning Stage</t>
+  </si>
+  <si>
+    <t>Log In Page - Front End</t>
+  </si>
+  <si>
+    <t>Index Page - unlogged in - Front end</t>
+  </si>
+  <si>
+    <t>Index Page - logged in - Front end</t>
+  </si>
+  <si>
+    <t>Add Stock  - Front end</t>
+  </si>
+  <si>
+    <t>Remove  Stock - Front end</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +219,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -164,7 +278,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -172,10 +286,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -511,33 +626,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.26953125" customWidth="1"/>
-    <col min="2" max="2" width="25.453125" customWidth="1"/>
-    <col min="3" max="3" width="36.81640625" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="36.77734375" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -548,51 +668,268 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="7">
+        <v>45569</v>
+      </c>
+      <c r="F14" s="7">
+        <v>45569</v>
+      </c>
+      <c r="G14" s="7">
+        <v>45569</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="7">
+        <v>45572</v>
+      </c>
+      <c r="F15" s="7">
+        <v>45578</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="7">
+        <v>45572</v>
+      </c>
+      <c r="F16" s="7">
+        <v>45578</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="7">
+        <v>45572</v>
+      </c>
+      <c r="F17" s="7">
+        <v>45578</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="7">
+        <v>45572</v>
+      </c>
+      <c r="F18" s="7">
+        <v>45578</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{A28441FA-4D61-47AD-8606-0100E29F3107}"/>
     <hyperlink ref="B7" r:id="rId2" xr:uid="{607FA25D-6CA6-4CDA-8769-F825536709F8}"/>

</xml_diff>